<commit_message>
modified:   baixar_imagens/Links.xlsx new file:   baixar_imagens/~$Links.xlsx new file:   easyprint.py
</commit_message>
<xml_diff>
--- a/baixar_imagens/Links.xlsx
+++ b/baixar_imagens/Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joab.alves\Desktop\automacoes_atacadao\baixar_imagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342266D1-BF31-4F1E-B06F-B1028A2F208F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF48B2E-4FCE-4FD1-BA9C-C7C9045AE36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E502FECC-261D-47F0-98EA-7DD680AD7C21}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>link</t>
   </si>
@@ -44,70 +44,31 @@
     <t>nome</t>
   </si>
   <si>
-    <t>VMM70074</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/70074.png</t>
-  </si>
-  <si>
-    <t>VMW30102</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/30102.png</t>
-  </si>
-  <si>
-    <t>VMW30109</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/30109.png</t>
-  </si>
-  <si>
-    <t>VMW30108</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/30108.png</t>
-  </si>
-  <si>
-    <t>VMM71002</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/71002.png</t>
-  </si>
-  <si>
-    <t>VMM70091</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/70091.png</t>
-  </si>
-  <si>
-    <t>VMM70088</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/70088.png</t>
-  </si>
-  <si>
-    <t>VMF50081</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/50081.png</t>
-  </si>
-  <si>
-    <t>VMV40087</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/40087.png</t>
-  </si>
-  <si>
-    <t>VMM70077</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/70077.png</t>
-  </si>
-  <si>
-    <t>VMV40085</t>
-  </si>
-  <si>
-    <t>https://vmvalman.com.br/wp-content/uploads/2019/09/40085.png</t>
+    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101051000%2Ejpg</t>
+  </si>
+  <si>
+    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101021640%2Ejpg</t>
+  </si>
+  <si>
+    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101041217%2Ejpg</t>
+  </si>
+  <si>
+    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101042728%2Ejpg</t>
+  </si>
+  <si>
+    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101021569%2Ejpg</t>
+  </si>
+  <si>
+    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101021836%2Ejpg</t>
+  </si>
+  <si>
+    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101043090%2Ejpg</t>
+  </si>
+  <si>
+    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101021526%2Ejpg</t>
+  </si>
+  <si>
+    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101023715%2Ejpg</t>
   </si>
 </sst>
 </file>
@@ -485,7 +446,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,91 +465,81 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>101051000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>101021640</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>101041217</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>101042728</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>101021569</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>101021836</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>101043090</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>101021526</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>101023715</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A11"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A12"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13"/>

</xml_diff>

<commit_message>
modified:   baixar_imagens/Links.xlsx modified:   deixar_nome_ate_60_caracteres.py new file:   teste2.py
</commit_message>
<xml_diff>
--- a/baixar_imagens/Links.xlsx
+++ b/baixar_imagens/Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joab.alves\Desktop\automacoes_atacadao\baixar_imagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF48B2E-4FCE-4FD1-BA9C-C7C9045AE36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536E5D06-B140-4E88-B6EC-B6CA0843CD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E502FECC-261D-47F0-98EA-7DD680AD7C21}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>link</t>
   </si>
@@ -44,31 +44,31 @@
     <t>nome</t>
   </si>
   <si>
-    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101051000%2Ejpg</t>
-  </si>
-  <si>
-    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101021640%2Ejpg</t>
-  </si>
-  <si>
-    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101041217%2Ejpg</t>
-  </si>
-  <si>
-    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101042728%2Ejpg</t>
-  </si>
-  <si>
-    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101021569%2Ejpg</t>
-  </si>
-  <si>
-    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101021836%2Ejpg</t>
-  </si>
-  <si>
-    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101043090%2Ejpg</t>
-  </si>
-  <si>
-    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101021526%2Ejpg</t>
-  </si>
-  <si>
-    <t>https://c123.com.br/bel-ar/FotoRetArq.asp?a=101023715%2Ejpg</t>
+    <t>https://www.ideia2001.com.br/catmobile/FotoMobRetArq.asp?cerq=226&amp;n=21989</t>
+  </si>
+  <si>
+    <t>https://www.ideia2001.com.br/catmobile/FotoMobRetArq.asp?cerq=226&amp;n=50261</t>
+  </si>
+  <si>
+    <t>https://www.ideia2001.com.br/catmobile/FotoMobRetArq.asp?cerq=226&amp;n=650158</t>
+  </si>
+  <si>
+    <t>https://www.ideia2001.com.br/catmobile/FotoMobRetArq.asp?cerq=226&amp;n=50193</t>
+  </si>
+  <si>
+    <t>https://www.ideia2001.com.br/catmobile/FotoMobRetArq.asp?cerq=226&amp;n=50282</t>
+  </si>
+  <si>
+    <t>https://www.ideia2001.com.br/catmobile/FotoMobRetArq.asp?cerq=226&amp;n=60124</t>
+  </si>
+  <si>
+    <t>https://www.ideia2001.com.br/catmobile/FotoMobRetArq.asp?cerq=226&amp;n=21503</t>
+  </si>
+  <si>
+    <t>https://www.ideia2001.com.br/catmobile/FotoMobRetArq.asp?cerq=226&amp;n=50127</t>
+  </si>
+  <si>
+    <t>https://www.ideia2001.com.br/catmobile/FotoMobRetArq.asp?cerq=226&amp;n=50195</t>
   </si>
 </sst>
 </file>
@@ -443,11 +443,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B3B02E-6FEB-4E48-A123-FFA1FD149E5A}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -455,7 +453,7 @@
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,94 +461,121 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>101051000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21989</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>101021640</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50261</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>101041217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>650158</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>101042728</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>101021569</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50282</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>101021836</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>101043090</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21503</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>101021526</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>101023715</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50195</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -609,5 +634,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>